<commit_message>
Replaced BUG REPORT.docx with and prj2.xlsx updated version
</commit_message>
<xml_diff>
--- a/Manual testing/Project2/prj2.xlsx
+++ b/Manual testing/Project2/prj2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Grow_Skills\Software testing\Manual testing\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B620977-7B7B-4BA1-8402-C46F091C89BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59184A8C-3FDB-4644-AF85-ECD486D155EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2F247890-709B-466F-AEF0-FBB19F461928}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>TEST SCENARIOS ID</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t xml:space="preserve">Verify the navigation behaviour Where2Go link </t>
+  </si>
+  <si>
+    <t>User needs to stay login and is on the MakeMyTrip home page</t>
   </si>
 </sst>
 </file>
@@ -248,7 +251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -279,6 +282,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -597,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03EBE9AF-13BB-4014-BAA3-B3C4F22E4445}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -661,7 +667,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>15</v>
@@ -692,8 +698,8 @@
       <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>12</v>
+      <c r="E3" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>21</v>
@@ -759,7 +765,7 @@
       <c r="E5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="11" t="s">
         <v>37</v>
       </c>
       <c r="G5" s="10" t="s">

</xml_diff>